<commit_message>
Update test script with test plan
</commit_message>
<xml_diff>
--- a/0WM_BLT3/Process/0WM_BLT3.xlsx
+++ b/0WM_BLT3/Process/0WM_BLT3.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -215,30 +215,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Speaker_L</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT3\Test_Speaker_L.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT3\log\Test_Speaker_L_CheckLog.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speaker_R</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT3\Test_Speaker_R.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C:\TestProgram\0WM\0WM_BLT3\log\Test_Speaker_R_CheckLog.bat</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>LED10to16</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -269,9 +245,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>XMOS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -301,6 +274,18 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT3\Test_Speaker.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:\TestProgram\0WM\0WM_BLT3\log\Test_Speaker_CheckLog.bat</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -688,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -784,22 +769,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>21</v>
@@ -813,22 +798,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>21</v>
@@ -950,7 +935,7 @@
         <v>4</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
@@ -979,7 +964,7 @@
         <v>21</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
@@ -1008,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.15">
@@ -1037,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.15">
@@ -1066,7 +1051,7 @@
         <v>21</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.15">
@@ -1074,86 +1059,57 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="M12" s="2">
         <v>4</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M13" s="2">
         <v>4</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="2">
-        <v>4</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>